<commit_message>
Add chin descriptors and add MQN .py
</commit_message>
<xml_diff>
--- a/docs/list_descriptor1D2D.xlsx
+++ b/docs/list_descriptor1D2D.xlsx
@@ -1,40 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borrela2\development\molecular-descriptors\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aborr\research\python_packages_dev\CompDESC\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524E5895-D4FD-4703-A369-DA81B8B7EFDB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B90333-66A7-4FFF-ADA0-61E7C45D33DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" tabRatio="684" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constitution" sheetId="1" r:id="rId1"/>
-    <sheet name="Molcular property" sheetId="2" r:id="rId2"/>
-    <sheet name="Topological" sheetId="3" r:id="rId3"/>
-    <sheet name="Connectivity" sheetId="4" r:id="rId4"/>
-    <sheet name="kappa" sheetId="5" r:id="rId5"/>
-    <sheet name="bcut" sheetId="6" r:id="rId6"/>
-    <sheet name="basak" sheetId="7" r:id="rId7"/>
-    <sheet name="Estate" sheetId="8" r:id="rId8"/>
-    <sheet name="Moreau-Broto autocorrelation" sheetId="9" r:id="rId9"/>
-    <sheet name="Moran autocorrelation" sheetId="10" r:id="rId10"/>
-    <sheet name="Morgan FP" sheetId="14" r:id="rId11"/>
-    <sheet name="Geary autocorelation" sheetId="11" r:id="rId12"/>
-    <sheet name="Charges" sheetId="12" r:id="rId13"/>
-    <sheet name="MOE" sheetId="13" r:id="rId14"/>
+    <sheet name="MQN" sheetId="15" r:id="rId2"/>
+    <sheet name="Molcular property" sheetId="2" r:id="rId3"/>
+    <sheet name="Topological" sheetId="3" r:id="rId4"/>
+    <sheet name="Connectivity" sheetId="4" r:id="rId5"/>
+    <sheet name="kappa" sheetId="5" r:id="rId6"/>
+    <sheet name="bcut" sheetId="6" r:id="rId7"/>
+    <sheet name="basak" sheetId="7" r:id="rId8"/>
+    <sheet name="Estate" sheetId="8" r:id="rId9"/>
+    <sheet name="Moreau-Broto autocorrelation" sheetId="9" r:id="rId10"/>
+    <sheet name="Moran autocorrelation" sheetId="10" r:id="rId11"/>
+    <sheet name="Morgan FP" sheetId="14" r:id="rId12"/>
+    <sheet name="Geary autocorelation" sheetId="11" r:id="rId13"/>
+    <sheet name="Charges" sheetId="12" r:id="rId14"/>
+    <sheet name="MOE" sheetId="13" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="1120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="1170">
   <si>
     <t>Constitutional</t>
   </si>
@@ -3394,13 +3394,163 @@
   </si>
   <si>
     <t>qed</t>
+  </si>
+  <si>
+    <t>NumLipinskiHBA</t>
+  </si>
+  <si>
+    <t>NumLipinskiHBD</t>
+  </si>
+  <si>
+    <t>NumStereocenters</t>
+  </si>
+  <si>
+    <t>NumUnspecifiedStereocenters</t>
+  </si>
+  <si>
+    <t>Molecular Quantum Numbers (MQN)</t>
+  </si>
+  <si>
+    <t>Added with the version 0.11 of compDesc</t>
+  </si>
+  <si>
+    <t>MQN1</t>
+  </si>
+  <si>
+    <t>MQN2</t>
+  </si>
+  <si>
+    <t>MQN3</t>
+  </si>
+  <si>
+    <t>MQN4</t>
+  </si>
+  <si>
+    <t>MQN5</t>
+  </si>
+  <si>
+    <t>MQN6</t>
+  </si>
+  <si>
+    <t>MQN7</t>
+  </si>
+  <si>
+    <t>MQN8</t>
+  </si>
+  <si>
+    <t>MQN9</t>
+  </si>
+  <si>
+    <t>MQN10</t>
+  </si>
+  <si>
+    <t>MQN11</t>
+  </si>
+  <si>
+    <t>MQN12</t>
+  </si>
+  <si>
+    <t>MQN13</t>
+  </si>
+  <si>
+    <t>MQN14</t>
+  </si>
+  <si>
+    <t>MQN15</t>
+  </si>
+  <si>
+    <t>MQN16</t>
+  </si>
+  <si>
+    <t>MQN17</t>
+  </si>
+  <si>
+    <t>MQN18</t>
+  </si>
+  <si>
+    <t>MQN19</t>
+  </si>
+  <si>
+    <t>MQN20</t>
+  </si>
+  <si>
+    <t>MQN21</t>
+  </si>
+  <si>
+    <t>MQN22</t>
+  </si>
+  <si>
+    <t>MQN23</t>
+  </si>
+  <si>
+    <t>MQN24</t>
+  </si>
+  <si>
+    <t>MQN25</t>
+  </si>
+  <si>
+    <t>MQN26</t>
+  </si>
+  <si>
+    <t>MQN27</t>
+  </si>
+  <si>
+    <t>MQN28</t>
+  </si>
+  <si>
+    <t>MQN29</t>
+  </si>
+  <si>
+    <t>MQN30</t>
+  </si>
+  <si>
+    <t>MQN31</t>
+  </si>
+  <si>
+    <t>MQN32</t>
+  </si>
+  <si>
+    <t>MQN33</t>
+  </si>
+  <si>
+    <t>MQN34</t>
+  </si>
+  <si>
+    <t>MQN35</t>
+  </si>
+  <si>
+    <t>MQN36</t>
+  </si>
+  <si>
+    <t>MQN37</t>
+  </si>
+  <si>
+    <t>MQN38</t>
+  </si>
+  <si>
+    <t>MQN39</t>
+  </si>
+  <si>
+    <t>MQN40</t>
+  </si>
+  <si>
+    <t>MQN41</t>
+  </si>
+  <si>
+    <t>MQN42</t>
+  </si>
+  <si>
+    <t>NumAmideBonds</t>
+  </si>
+  <si>
+    <t>Added with the version 0.9 of compDesc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3422,6 +3572,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3776,10 +3932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4427,13 +4583,693 @@
         <v>69</v>
       </c>
     </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>1120</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>1121</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>1122</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1169</v>
+      </c>
+      <c r="F46" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4283E985-4A18-4525-904E-F38821CBAA2F}">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="C1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>806</v>
+      </c>
+      <c r="B3">
+        <v>3.9918330000000002</v>
+      </c>
+      <c r="C3" t="s">
+        <v>846</v>
+      </c>
+      <c r="D3">
+        <v>3.9918330000000002</v>
+      </c>
+      <c r="E3" t="s">
+        <v>840</v>
+      </c>
+      <c r="F3" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>807</v>
+      </c>
+      <c r="B4">
+        <v>4.3588630000000004</v>
+      </c>
+      <c r="C4" t="s">
+        <v>847</v>
+      </c>
+      <c r="D4">
+        <v>4.3588630000000004</v>
+      </c>
+      <c r="E4" t="s">
+        <v>841</v>
+      </c>
+      <c r="F4" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>808</v>
+      </c>
+      <c r="B5">
+        <v>4.39405</v>
+      </c>
+      <c r="C5" t="s">
+        <v>848</v>
+      </c>
+      <c r="D5">
+        <v>4.39405</v>
+      </c>
+      <c r="E5" t="s">
+        <v>842</v>
+      </c>
+      <c r="F5" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>809</v>
+      </c>
+      <c r="B6">
+        <v>4.3808569999999998</v>
+      </c>
+      <c r="C6" t="s">
+        <v>849</v>
+      </c>
+      <c r="D6">
+        <v>4.3808569999999998</v>
+      </c>
+      <c r="E6" t="s">
+        <v>843</v>
+      </c>
+      <c r="F6" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>810</v>
+      </c>
+      <c r="B7">
+        <v>4.3365109999999998</v>
+      </c>
+      <c r="C7" t="s">
+        <v>850</v>
+      </c>
+      <c r="D7">
+        <v>4.3365109999999998</v>
+      </c>
+      <c r="E7" t="s">
+        <v>844</v>
+      </c>
+      <c r="F7" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>811</v>
+      </c>
+      <c r="B8">
+        <v>4.4076110000000002</v>
+      </c>
+      <c r="C8" t="s">
+        <v>851</v>
+      </c>
+      <c r="D8">
+        <v>4.4076110000000002</v>
+      </c>
+      <c r="E8" t="s">
+        <v>845</v>
+      </c>
+      <c r="F8" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>812</v>
+      </c>
+      <c r="B9">
+        <v>4.4291080000000003</v>
+      </c>
+      <c r="C9" t="s">
+        <v>852</v>
+      </c>
+      <c r="D9">
+        <v>4.4291080000000003</v>
+      </c>
+      <c r="E9" t="s">
+        <v>880</v>
+      </c>
+      <c r="F9" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>813</v>
+      </c>
+      <c r="B10">
+        <v>4.4526269999999997</v>
+      </c>
+      <c r="C10" t="s">
+        <v>853</v>
+      </c>
+      <c r="D10">
+        <v>4.4526269999999997</v>
+      </c>
+      <c r="E10" t="s">
+        <v>879</v>
+      </c>
+      <c r="F10" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>814</v>
+      </c>
+      <c r="B11">
+        <v>3.7077429999999998</v>
+      </c>
+      <c r="C11" t="s">
+        <v>854</v>
+      </c>
+      <c r="D11">
+        <v>3.7077429999999998</v>
+      </c>
+      <c r="E11" t="s">
+        <v>881</v>
+      </c>
+      <c r="F11" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>815</v>
+      </c>
+      <c r="B12">
+        <v>3.989185</v>
+      </c>
+      <c r="C12" t="s">
+        <v>855</v>
+      </c>
+      <c r="D12">
+        <v>3.989185</v>
+      </c>
+      <c r="F12" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>816</v>
+      </c>
+      <c r="B13">
+        <v>3.9416690000000001</v>
+      </c>
+      <c r="C13" t="s">
+        <v>856</v>
+      </c>
+      <c r="D13">
+        <v>3.9416690000000001</v>
+      </c>
+      <c r="F13" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>817</v>
+      </c>
+      <c r="B14">
+        <v>3.8447249999999999</v>
+      </c>
+      <c r="C14" t="s">
+        <v>857</v>
+      </c>
+      <c r="D14">
+        <v>3.8447249999999999</v>
+      </c>
+      <c r="F14" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>818</v>
+      </c>
+      <c r="B15">
+        <v>3.8779849999999998</v>
+      </c>
+      <c r="C15" t="s">
+        <v>858</v>
+      </c>
+      <c r="D15">
+        <v>3.8779849999999998</v>
+      </c>
+      <c r="F15" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>819</v>
+      </c>
+      <c r="B16">
+        <v>3.9451749999999999</v>
+      </c>
+      <c r="C16" t="s">
+        <v>859</v>
+      </c>
+      <c r="D16">
+        <v>3.9451749999999999</v>
+      </c>
+      <c r="F16" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>820</v>
+      </c>
+      <c r="B17">
+        <v>3.9965579999999998</v>
+      </c>
+      <c r="C17" t="s">
+        <v>860</v>
+      </c>
+      <c r="D17">
+        <v>3.9965579999999998</v>
+      </c>
+      <c r="F17" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>821</v>
+      </c>
+      <c r="B18">
+        <v>4.0100410000000002</v>
+      </c>
+      <c r="C18" t="s">
+        <v>861</v>
+      </c>
+      <c r="D18">
+        <v>4.0100410000000002</v>
+      </c>
+      <c r="F18" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>822</v>
+      </c>
+      <c r="B19">
+        <v>3.9895900000000002</v>
+      </c>
+      <c r="C19" t="s">
+        <v>862</v>
+      </c>
+      <c r="D19">
+        <v>3.9895900000000002</v>
+      </c>
+      <c r="E19" t="s">
+        <v>882</v>
+      </c>
+      <c r="F19" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>823</v>
+      </c>
+      <c r="B20">
+        <v>4.3556499999999998</v>
+      </c>
+      <c r="C20" t="s">
+        <v>863</v>
+      </c>
+      <c r="D20">
+        <v>4.3556499999999998</v>
+      </c>
+      <c r="F20" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>824</v>
+      </c>
+      <c r="B21">
+        <v>4.3907340000000001</v>
+      </c>
+      <c r="C21" t="s">
+        <v>864</v>
+      </c>
+      <c r="D21">
+        <v>4.3907340000000001</v>
+      </c>
+      <c r="F21" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>825</v>
+      </c>
+      <c r="B22">
+        <v>4.3768649999999996</v>
+      </c>
+      <c r="C22" t="s">
+        <v>865</v>
+      </c>
+      <c r="D22">
+        <v>4.3768649999999996</v>
+      </c>
+      <c r="F22" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>826</v>
+      </c>
+      <c r="B23">
+        <v>4.3332829999999998</v>
+      </c>
+      <c r="C23" t="s">
+        <v>866</v>
+      </c>
+      <c r="D23">
+        <v>4.3332829999999998</v>
+      </c>
+      <c r="F23" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>827</v>
+      </c>
+      <c r="B24">
+        <v>4.4041090000000001</v>
+      </c>
+      <c r="C24" t="s">
+        <v>867</v>
+      </c>
+      <c r="D24">
+        <v>4.4041090000000001</v>
+      </c>
+      <c r="F24" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>828</v>
+      </c>
+      <c r="B25">
+        <v>4.4260260000000002</v>
+      </c>
+      <c r="C25" t="s">
+        <v>868</v>
+      </c>
+      <c r="D25">
+        <v>4.4260260000000002</v>
+      </c>
+      <c r="F25" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>829</v>
+      </c>
+      <c r="B26">
+        <v>4.4493859999999996</v>
+      </c>
+      <c r="C26" t="s">
+        <v>869</v>
+      </c>
+      <c r="D26">
+        <v>4.4493859999999996</v>
+      </c>
+      <c r="F26" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>830</v>
+      </c>
+      <c r="B27">
+        <v>3.6742849999999998</v>
+      </c>
+      <c r="C27" t="s">
+        <v>870</v>
+      </c>
+      <c r="D27">
+        <v>3.6742849999999998</v>
+      </c>
+      <c r="E27" t="s">
+        <v>883</v>
+      </c>
+      <c r="F27" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>831</v>
+      </c>
+      <c r="B28">
+        <v>3.9521700000000002</v>
+      </c>
+      <c r="C28" t="s">
+        <v>871</v>
+      </c>
+      <c r="D28">
+        <v>3.9521700000000002</v>
+      </c>
+      <c r="F28" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>832</v>
+      </c>
+      <c r="B29">
+        <v>3.8906860000000001</v>
+      </c>
+      <c r="C29" t="s">
+        <v>872</v>
+      </c>
+      <c r="D29">
+        <v>3.8906860000000001</v>
+      </c>
+      <c r="F29" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>833</v>
+      </c>
+      <c r="B30">
+        <v>3.7875239999999999</v>
+      </c>
+      <c r="C30" t="s">
+        <v>873</v>
+      </c>
+      <c r="D30">
+        <v>3.7875239999999999</v>
+      </c>
+      <c r="F30" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>834</v>
+      </c>
+      <c r="B31">
+        <v>3.8270930000000001</v>
+      </c>
+      <c r="C31" t="s">
+        <v>874</v>
+      </c>
+      <c r="D31">
+        <v>3.8270930000000001</v>
+      </c>
+      <c r="F31" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>835</v>
+      </c>
+      <c r="B32">
+        <v>3.899842</v>
+      </c>
+      <c r="C32" t="s">
+        <v>875</v>
+      </c>
+      <c r="D32">
+        <v>3.899842</v>
+      </c>
+      <c r="F32" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>836</v>
+      </c>
+      <c r="B33">
+        <v>3.9490560000000001</v>
+      </c>
+      <c r="C33" t="s">
+        <v>876</v>
+      </c>
+      <c r="D33">
+        <v>3.9490560000000001</v>
+      </c>
+      <c r="F33" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>837</v>
+      </c>
+      <c r="B34">
+        <v>3.964388</v>
+      </c>
+      <c r="C34" t="s">
+        <v>877</v>
+      </c>
+      <c r="D34">
+        <v>3.964388</v>
+      </c>
+      <c r="F34" t="s">
+        <v>878</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B1A4C5-DD22-4302-AD1C-8537DC117209}">
   <dimension ref="A1:F34"/>
   <sheetViews>
@@ -4943,7 +5779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FBC61CA-6294-4444-914C-F6EEBA5EB2E6}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -5020,7 +5856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EE91B9-2151-4DED-8739-892DB78E1E96}">
   <dimension ref="A1:F34"/>
   <sheetViews>
@@ -5530,7 +6366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5A38F9-2833-4516-A297-DA618F3FC5B5}">
   <dimension ref="A1:H31"/>
   <sheetViews>
@@ -6008,12 +6844,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E561671C-2D8B-419F-8325-AE72F69A5B09}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6995,11 +7831,517 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB6E21CF-11B5-45DD-9290-A478974E4AFB}">
+  <dimension ref="A1:F44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>1130</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E41" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>1166</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>1167</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7214,12 +8556,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7696,12 +9038,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86D9B3E-6761-4EC5-BC24-988202167197}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8284,12 +9626,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5669C31E-62DC-4D85-A64E-E0B4A29701C2}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="B3" sqref="B3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8482,11 +9824,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72858A2C-2AA5-472D-AF80-6EFF17405DD1}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
@@ -9442,7 +10784,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311BC8BE-1294-4485-8840-E8D10724D4F9}">
   <dimension ref="A1:G23"/>
   <sheetViews>
@@ -9766,11 +11108,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16169526-9B51-4495-9715-07B3E3E4FE8E}">
   <dimension ref="A1:F332"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E173" sqref="E173"/>
     </sheetView>
   </sheetViews>
@@ -13898,629 +15240,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4283E985-4A18-4525-904E-F38821CBAA2F}">
-  <dimension ref="A1:F34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="46.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>805</v>
-      </c>
-      <c r="C1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>806</v>
-      </c>
-      <c r="B3">
-        <v>3.9918330000000002</v>
-      </c>
-      <c r="C3" t="s">
-        <v>846</v>
-      </c>
-      <c r="D3">
-        <v>3.9918330000000002</v>
-      </c>
-      <c r="E3" t="s">
-        <v>840</v>
-      </c>
-      <c r="F3" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>807</v>
-      </c>
-      <c r="B4">
-        <v>4.3588630000000004</v>
-      </c>
-      <c r="C4" t="s">
-        <v>847</v>
-      </c>
-      <c r="D4">
-        <v>4.3588630000000004</v>
-      </c>
-      <c r="E4" t="s">
-        <v>841</v>
-      </c>
-      <c r="F4" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>808</v>
-      </c>
-      <c r="B5">
-        <v>4.39405</v>
-      </c>
-      <c r="C5" t="s">
-        <v>848</v>
-      </c>
-      <c r="D5">
-        <v>4.39405</v>
-      </c>
-      <c r="E5" t="s">
-        <v>842</v>
-      </c>
-      <c r="F5" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>809</v>
-      </c>
-      <c r="B6">
-        <v>4.3808569999999998</v>
-      </c>
-      <c r="C6" t="s">
-        <v>849</v>
-      </c>
-      <c r="D6">
-        <v>4.3808569999999998</v>
-      </c>
-      <c r="E6" t="s">
-        <v>843</v>
-      </c>
-      <c r="F6" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>810</v>
-      </c>
-      <c r="B7">
-        <v>4.3365109999999998</v>
-      </c>
-      <c r="C7" t="s">
-        <v>850</v>
-      </c>
-      <c r="D7">
-        <v>4.3365109999999998</v>
-      </c>
-      <c r="E7" t="s">
-        <v>844</v>
-      </c>
-      <c r="F7" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>811</v>
-      </c>
-      <c r="B8">
-        <v>4.4076110000000002</v>
-      </c>
-      <c r="C8" t="s">
-        <v>851</v>
-      </c>
-      <c r="D8">
-        <v>4.4076110000000002</v>
-      </c>
-      <c r="E8" t="s">
-        <v>845</v>
-      </c>
-      <c r="F8" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>812</v>
-      </c>
-      <c r="B9">
-        <v>4.4291080000000003</v>
-      </c>
-      <c r="C9" t="s">
-        <v>852</v>
-      </c>
-      <c r="D9">
-        <v>4.4291080000000003</v>
-      </c>
-      <c r="E9" t="s">
-        <v>880</v>
-      </c>
-      <c r="F9" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>813</v>
-      </c>
-      <c r="B10">
-        <v>4.4526269999999997</v>
-      </c>
-      <c r="C10" t="s">
-        <v>853</v>
-      </c>
-      <c r="D10">
-        <v>4.4526269999999997</v>
-      </c>
-      <c r="E10" t="s">
-        <v>879</v>
-      </c>
-      <c r="F10" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>814</v>
-      </c>
-      <c r="B11">
-        <v>3.7077429999999998</v>
-      </c>
-      <c r="C11" t="s">
-        <v>854</v>
-      </c>
-      <c r="D11">
-        <v>3.7077429999999998</v>
-      </c>
-      <c r="E11" t="s">
-        <v>881</v>
-      </c>
-      <c r="F11" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>815</v>
-      </c>
-      <c r="B12">
-        <v>3.989185</v>
-      </c>
-      <c r="C12" t="s">
-        <v>855</v>
-      </c>
-      <c r="D12">
-        <v>3.989185</v>
-      </c>
-      <c r="F12" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>816</v>
-      </c>
-      <c r="B13">
-        <v>3.9416690000000001</v>
-      </c>
-      <c r="C13" t="s">
-        <v>856</v>
-      </c>
-      <c r="D13">
-        <v>3.9416690000000001</v>
-      </c>
-      <c r="F13" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>817</v>
-      </c>
-      <c r="B14">
-        <v>3.8447249999999999</v>
-      </c>
-      <c r="C14" t="s">
-        <v>857</v>
-      </c>
-      <c r="D14">
-        <v>3.8447249999999999</v>
-      </c>
-      <c r="F14" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>818</v>
-      </c>
-      <c r="B15">
-        <v>3.8779849999999998</v>
-      </c>
-      <c r="C15" t="s">
-        <v>858</v>
-      </c>
-      <c r="D15">
-        <v>3.8779849999999998</v>
-      </c>
-      <c r="F15" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>819</v>
-      </c>
-      <c r="B16">
-        <v>3.9451749999999999</v>
-      </c>
-      <c r="C16" t="s">
-        <v>859</v>
-      </c>
-      <c r="D16">
-        <v>3.9451749999999999</v>
-      </c>
-      <c r="F16" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>820</v>
-      </c>
-      <c r="B17">
-        <v>3.9965579999999998</v>
-      </c>
-      <c r="C17" t="s">
-        <v>860</v>
-      </c>
-      <c r="D17">
-        <v>3.9965579999999998</v>
-      </c>
-      <c r="F17" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>821</v>
-      </c>
-      <c r="B18">
-        <v>4.0100410000000002</v>
-      </c>
-      <c r="C18" t="s">
-        <v>861</v>
-      </c>
-      <c r="D18">
-        <v>4.0100410000000002</v>
-      </c>
-      <c r="F18" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>822</v>
-      </c>
-      <c r="B19">
-        <v>3.9895900000000002</v>
-      </c>
-      <c r="C19" t="s">
-        <v>862</v>
-      </c>
-      <c r="D19">
-        <v>3.9895900000000002</v>
-      </c>
-      <c r="E19" t="s">
-        <v>882</v>
-      </c>
-      <c r="F19" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>823</v>
-      </c>
-      <c r="B20">
-        <v>4.3556499999999998</v>
-      </c>
-      <c r="C20" t="s">
-        <v>863</v>
-      </c>
-      <c r="D20">
-        <v>4.3556499999999998</v>
-      </c>
-      <c r="F20" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>824</v>
-      </c>
-      <c r="B21">
-        <v>4.3907340000000001</v>
-      </c>
-      <c r="C21" t="s">
-        <v>864</v>
-      </c>
-      <c r="D21">
-        <v>4.3907340000000001</v>
-      </c>
-      <c r="F21" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>825</v>
-      </c>
-      <c r="B22">
-        <v>4.3768649999999996</v>
-      </c>
-      <c r="C22" t="s">
-        <v>865</v>
-      </c>
-      <c r="D22">
-        <v>4.3768649999999996</v>
-      </c>
-      <c r="F22" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>826</v>
-      </c>
-      <c r="B23">
-        <v>4.3332829999999998</v>
-      </c>
-      <c r="C23" t="s">
-        <v>866</v>
-      </c>
-      <c r="D23">
-        <v>4.3332829999999998</v>
-      </c>
-      <c r="F23" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>827</v>
-      </c>
-      <c r="B24">
-        <v>4.4041090000000001</v>
-      </c>
-      <c r="C24" t="s">
-        <v>867</v>
-      </c>
-      <c r="D24">
-        <v>4.4041090000000001</v>
-      </c>
-      <c r="F24" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>828</v>
-      </c>
-      <c r="B25">
-        <v>4.4260260000000002</v>
-      </c>
-      <c r="C25" t="s">
-        <v>868</v>
-      </c>
-      <c r="D25">
-        <v>4.4260260000000002</v>
-      </c>
-      <c r="F25" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>829</v>
-      </c>
-      <c r="B26">
-        <v>4.4493859999999996</v>
-      </c>
-      <c r="C26" t="s">
-        <v>869</v>
-      </c>
-      <c r="D26">
-        <v>4.4493859999999996</v>
-      </c>
-      <c r="F26" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>830</v>
-      </c>
-      <c r="B27">
-        <v>3.6742849999999998</v>
-      </c>
-      <c r="C27" t="s">
-        <v>870</v>
-      </c>
-      <c r="D27">
-        <v>3.6742849999999998</v>
-      </c>
-      <c r="E27" t="s">
-        <v>883</v>
-      </c>
-      <c r="F27" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>831</v>
-      </c>
-      <c r="B28">
-        <v>3.9521700000000002</v>
-      </c>
-      <c r="C28" t="s">
-        <v>871</v>
-      </c>
-      <c r="D28">
-        <v>3.9521700000000002</v>
-      </c>
-      <c r="F28" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>832</v>
-      </c>
-      <c r="B29">
-        <v>3.8906860000000001</v>
-      </c>
-      <c r="C29" t="s">
-        <v>872</v>
-      </c>
-      <c r="D29">
-        <v>3.8906860000000001</v>
-      </c>
-      <c r="F29" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>833</v>
-      </c>
-      <c r="B30">
-        <v>3.7875239999999999</v>
-      </c>
-      <c r="C30" t="s">
-        <v>873</v>
-      </c>
-      <c r="D30">
-        <v>3.7875239999999999</v>
-      </c>
-      <c r="F30" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>834</v>
-      </c>
-      <c r="B31">
-        <v>3.8270930000000001</v>
-      </c>
-      <c r="C31" t="s">
-        <v>874</v>
-      </c>
-      <c r="D31">
-        <v>3.8270930000000001</v>
-      </c>
-      <c r="F31" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>835</v>
-      </c>
-      <c r="B32">
-        <v>3.899842</v>
-      </c>
-      <c r="C32" t="s">
-        <v>875</v>
-      </c>
-      <c r="D32">
-        <v>3.899842</v>
-      </c>
-      <c r="F32" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>836</v>
-      </c>
-      <c r="B33">
-        <v>3.9490560000000001</v>
-      </c>
-      <c r="C33" t="s">
-        <v>876</v>
-      </c>
-      <c r="D33">
-        <v>3.9490560000000001</v>
-      </c>
-      <c r="F33" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>837</v>
-      </c>
-      <c r="B34">
-        <v>3.964388</v>
-      </c>
-      <c r="C34" t="s">
-        <v>877</v>
-      </c>
-      <c r="D34">
-        <v>3.964388</v>
-      </c>
-      <c r="F34" t="s">
-        <v>878</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>